<commit_message>
update writer for comments and m-number
</commit_message>
<xml_diff>
--- a/Excel_templates/Input_file_template.xlsx
+++ b/Excel_templates/Input_file_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Web Development\Random Projects\CPI_Projects\240715_PRS_Excel\Excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B84DAF7-D14E-4229-A447-136A39FAC39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5CDBAA-4D36-41E1-81AE-062B4EA247D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Item</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>GIC - 82203</t>
+  </si>
+  <si>
+    <t>M-number (optional)</t>
+  </si>
+  <si>
+    <t>M-1234</t>
+  </si>
+  <si>
+    <t>Quoted 50% off with code (1234)</t>
+  </si>
+  <si>
+    <t>Additional Comments (optional)</t>
   </si>
 </sst>
 </file>
@@ -396,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,11 +420,13 @@
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,14 +448,20 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -463,14 +483,21 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
         <v>50</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>200</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>